<commit_message>
Prepare for release 1.2
Labelling, part names and numbers, new Gerbers and production documents
</commit_message>
<xml_diff>
--- a/POSCON.PCB Production Files/POSCON.PCB.ECO.xlsx
+++ b/POSCON.PCB Production Files/POSCON.PCB.ECO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Change</t>
   </si>
@@ -43,6 +43,39 @@
   </si>
   <si>
     <t>Rafael Send</t>
+  </si>
+  <si>
+    <t>POSCON.PCB.v1.1</t>
+  </si>
+  <si>
+    <t>POSCON.PCB.v1.2</t>
+  </si>
+  <si>
+    <t>Power trace</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>New MCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased size of power trace </t>
+  </si>
+  <si>
+    <t>Changed MCU to MC9S08SH8CTG</t>
+  </si>
+  <si>
+    <t>Changed mechanical drawings in top level, incorrect tag for PCB</t>
+  </si>
+  <si>
+    <t>Changed 7Segment resistor arrays to 620Ohm</t>
+  </si>
+  <si>
+    <t>Vias tented</t>
+  </si>
+  <si>
+    <t>Changed Eagle setting to tent vias in design, not at manufacturer.</t>
   </si>
 </sst>
 </file>
@@ -391,18 +424,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -438,6 +471,70 @@
       </c>
       <c r="E2" s="2">
         <v>41926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New files for release 1.2
For review and sent to quote at AC.
</commit_message>
<xml_diff>
--- a/POSCON.PCB Production Files/POSCON.PCB.ECO.xlsx
+++ b/POSCON.PCB Production Files/POSCON.PCB.ECO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Change</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Changed Eagle setting to tent vias in design, not at manufacturer.</t>
+  </si>
+  <si>
+    <t>Fix silkscreen</t>
+  </si>
+  <si>
+    <t>Silkscreen overlapping pads usually ok for production but causes errors in DRC</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,7 +441,7 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,7 +507,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>42010</v>
+        <v>42014</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,6 +542,18 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>